<commit_message>
logger class is added
</commit_message>
<xml_diff>
--- a/src/main/com/com/framework/testdata/TestSuite1.xlsx
+++ b/src/main/com/com/framework/testdata/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19875" windowHeight="3240" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19875" windowHeight="3240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>TCID</t>
   </si>
@@ -99,7 +99,10 @@
     <t>verifyText</t>
   </si>
   <si>
-    <t>Jakay N</t>
+    <t>Jakay M</t>
+  </si>
+  <si>
+    <t>close</t>
   </si>
   <si>
     <t>Executed</t>
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +586,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -599,7 +602,7 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -617,7 +620,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -635,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -651,7 +654,7 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -668,11 +671,27 @@
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId7"/>
+    <hyperlink ref="D3" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -683,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,8 +758,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId12"/>
-    <hyperlink ref="C3" r:id="rId13"/>
+    <hyperlink ref="B3" r:id="rId30"/>
+    <hyperlink ref="C3" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>

</xml_diff>

<commit_message>
hard code values has been changed
</commit_message>
<xml_diff>
--- a/src/main/com/com/framework/testdata/TestSuite1.xlsx
+++ b/src/main/com/com/framework/testdata/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19875" windowHeight="3240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19875" windowHeight="3240"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>TCID</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>login_user_name</t>
   </si>
   <si>
@@ -106,14 +103,16 @@
   </si>
   <si>
     <t>Executed</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,15 +496,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="58.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="1" max="1" width="40.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="58.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,7 +526,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -539,18 +538,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="76.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.04833984375" collapsed="true"/>
+    <col min="1" max="1" width="41.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="76.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -586,7 +585,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -602,7 +601,7 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -620,7 +619,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -638,7 +637,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -654,7 +653,7 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -663,16 +662,16 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,17 +680,17 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId16"/>
+    <hyperlink ref="D3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -703,18 +702,18 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="47.0" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" hidden="true" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -750,16 +749,13 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId30"/>
-    <hyperlink ref="C3" r:id="rId31"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>

</xml_diff>